<commit_message>
update guide to make unit test for new feature
</commit_message>
<xml_diff>
--- a/gamble-doc.xlsx
+++ b/gamble-doc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUAN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUAN\Desktop\easy_tx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="value in shared memory" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="117">
   <si>
     <t>Tên biến</t>
   </si>
@@ -578,16 +578,25 @@
     <t>int8_t runAct(uint16_t money, NUT_TYPE type)\</t>
   </si>
   <si>
-    <t>int8_t setPoint()</t>
-  </si>
-  <si>
-    <t>Cài đặt contr chuột tới 1 vị trí chỉ đnh</t>
-  </si>
-  <si>
     <t xml:space="preserve">int8_t click() </t>
   </si>
   <si>
     <t>Thực hiện 1 lệnh click chuột, lệnh này yêu cầu click (giữ 100ms) và nhả chuột reuturn 1</t>
+  </si>
+  <si>
+    <t>int8_t setPoint(NUT_TYPE type)</t>
+  </si>
+  <si>
+    <t>Cài đặt contr chuột tới 1 vị trí chỉ đnh với NUT_TYPE là enum chỉ định vị trí tài hoặc xỉu</t>
+  </si>
+  <si>
+    <t>{
+{0,0},
+{0,0},
+{0,0},
+{0,0},
+{0,0}
+}</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,8 +1201,8 @@
       <c r="C7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="3">
-        <v>0</v>
+      <c r="D7" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>68</v>
@@ -1516,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2081,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,18 +2147,18 @@
         <v>29</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>